<commit_message>
Validar usuario y login
</commit_message>
<xml_diff>
--- a/CASO-VENTAS-PARA-TODOS.xlsx
+++ b/CASO-VENTAS-PARA-TODOS.xlsx
@@ -77,9 +77,6 @@
     <t>unidadMed</t>
   </si>
   <si>
-    <t>categoria</t>
-  </si>
-  <si>
     <t>precioUnit</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>telefono</t>
+  </si>
+  <si>
+    <t>usuario</t>
   </si>
 </sst>
 </file>
@@ -183,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +214,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -288,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -299,6 +305,16 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -311,16 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,38 +624,38 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="14"/>
+      <c r="J4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10"/>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -658,28 +665,28 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
+      <c r="G5" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="L5" s="1">
         <v>123456</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
@@ -708,15 +715,15 @@
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -740,10 +747,10 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
@@ -796,7 +803,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="2"/>
       <c r="N11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -808,12 +815,12 @@
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
       <c r="N12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
@@ -823,48 +830,48 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="10"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="F17" s="1" t="s">
+      <c r="C17" s="14"/>
+      <c r="F17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>40</v>
+      <c r="B18" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G18" s="1">
         <v>43631917</v>
@@ -908,12 +915,12 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="N20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="14"/>
+      <c r="N20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="11"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -924,17 +931,17 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
-      <c r="N21" s="15" t="s">
+      <c r="N21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="P21" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="O21" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="P21" s="15" t="s">
+      <c r="Q21" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="Q21" s="15" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
@@ -1002,15 +1009,15 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="D28" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1018,25 +1025,25 @@
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F29" s="16" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="3" t="s">
+      <c r="I29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I29" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="J29" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1045,10 +1052,10 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>6</v>
@@ -1074,13 +1081,13 @@
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G31" s="1">
         <f>D7+D7*E7</f>
@@ -1156,12 +1163,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D28:J28"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="F16:K16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B4:H4"/>
     <mergeCell ref="J3:M3"/>
-    <mergeCell ref="D28:J28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reporte de Ventas por fechas y pintado en colores
</commit_message>
<xml_diff>
--- a/CASO-VENTAS-PARA-TODOS.xlsx
+++ b/CASO-VENTAS-PARA-TODOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Productos</t>
   </si>
@@ -168,6 +168,18 @@
   </si>
   <si>
     <t>usuario</t>
+  </si>
+  <si>
+    <t>Reporte de Productos por stock</t>
+  </si>
+  <si>
+    <t>Reporte de Productos mas vendidos</t>
+  </si>
+  <si>
+    <t>Se debe agregar la funcionalidad de agregar stock, al momento de la venta debe disminuir el stock</t>
+  </si>
+  <si>
+    <t>Reporte de Ventas entre un rango de fechas</t>
   </si>
 </sst>
 </file>
@@ -183,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -306,6 +324,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -324,10 +346,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Q36"/>
+  <dimension ref="B3:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4:M4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,23 +643,23 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
       <c r="J4" s="1" t="s">
         <v>24</v>
       </c>
@@ -655,7 +674,7 @@
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -670,7 +689,7 @@
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -830,21 +849,21 @@
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="F17" s="16" t="s">
+      <c r="C17" s="16"/>
+      <c r="F17" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -864,7 +883,7 @@
       </c>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -915,12 +934,12 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
-      <c r="N20" s="9" t="s">
+      <c r="N20" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="11"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="13"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -1009,15 +1028,15 @@
       <c r="Q27" s="1"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -1027,10 +1046,10 @@
       <c r="D29" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="16" t="s">
+      <c r="E29" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="9" t="s">
         <v>12</v>
       </c>
       <c r="G29" s="7" t="s">
@@ -1161,14 +1180,32 @@
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
+    <row r="41" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D41" s="17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="4:17" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H44" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="J3:M3"/>
     <mergeCell ref="D28:J28"/>
     <mergeCell ref="N20:Q20"/>
     <mergeCell ref="F16:K16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B4:H4"/>
-    <mergeCell ref="J3:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>